<commit_message>
#remove stopwords remove _ 59,20% on unigram
</commit_message>
<xml_diff>
--- a/data/emoticon-emoji.xlsx
+++ b/data/emoticon-emoji.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1.UIT\Nam 4\Hoc ky 2\Khai thac du lieu truyen thong xa hoi - IE403.K21\1. Preprocessing Data\1. Emoji handling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1.UIT\Nam 4\Hoc ky 2\Khai thac du lieu truyen thong xa hoi - IE403.K21\Nhom3-15520395-15520632-15520710-16520568\Source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2731A62-F837-443C-B3F1-8C41AAE2C459}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DF1663-4E2D-481D-8CE6-841B5DA10C4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{9A3FB480-DDD1-4F21-8FE8-5E3D214F94A5}"/>
   </bookViews>
@@ -147,39 +147,6 @@
     <t>&gt;&lt;</t>
   </si>
   <si>
-    <t>:face_with_tongue:</t>
-  </si>
-  <si>
-    <t>:upside-down_face:</t>
-  </si>
-  <si>
-    <t>:expressionless_face:</t>
-  </si>
-  <si>
-    <t>:crying_face:</t>
-  </si>
-  <si>
-    <t>:face_with_tears_of_joy:</t>
-  </si>
-  <si>
-    <t>:grinning_squinting_face:</t>
-  </si>
-  <si>
-    <t>:slightly_smiling_face:</t>
-  </si>
-  <si>
-    <t>:frowning_face:</t>
-  </si>
-  <si>
-    <t>:confused_face:</t>
-  </si>
-  <si>
-    <t>:smiling_face_with_smiling_eyes:</t>
-  </si>
-  <si>
-    <t>:rolling_on_the_floor_laughing:</t>
-  </si>
-  <si>
     <t>=.=</t>
   </si>
   <si>
@@ -187,6 +154,39 @@
   </si>
   <si>
     <t>=)</t>
+  </si>
+  <si>
+    <t>lè lưỡi</t>
+  </si>
+  <si>
+    <t>cười lăn lộn</t>
+  </si>
+  <si>
+    <t>cười mĩm</t>
+  </si>
+  <si>
+    <t>cười</t>
+  </si>
+  <si>
+    <t>cười ra nước mắt</t>
+  </si>
+  <si>
+    <t>cảm thấy buồn</t>
+  </si>
+  <si>
+    <t>muốn khóc</t>
+  </si>
+  <si>
+    <t>mặt nhăn</t>
+  </si>
+  <si>
+    <t>rối rắm</t>
+  </si>
+  <si>
+    <t>cạn lời</t>
+  </si>
+  <si>
+    <t>cười híp mắt</t>
   </si>
 </sst>
 </file>
@@ -541,43 +541,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32D59E8-1448-4C4E-B064-503838A9CF24}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
@@ -609,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
@@ -678,7 +680,7 @@
         <v>25</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -714,7 +716,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Using emo-vietname_3 59,53% - 61,67%
</commit_message>
<xml_diff>
--- a/data/emoticon-emoji.xlsx
+++ b/data/emoticon-emoji.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1.UIT\Nam 4\Hoc ky 2\Khai thac du lieu truyen thong xa hoi - IE403.K21\Nhom3-15520395-15520632-15520710-16520568\Source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DF1663-4E2D-481D-8CE6-841B5DA10C4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A73BB9E-AA3A-48D1-949D-A6D1AC7D400E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{9A3FB480-DDD1-4F21-8FE8-5E3D214F94A5}"/>
   </bookViews>
@@ -159,15 +159,9 @@
     <t>lè lưỡi</t>
   </si>
   <si>
-    <t>cười lăn lộn</t>
-  </si>
-  <si>
     <t>cười mĩm</t>
   </si>
   <si>
-    <t>cười</t>
-  </si>
-  <si>
     <t>cười ra nước mắt</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>muốn khóc</t>
   </si>
   <si>
-    <t>mặt nhăn</t>
-  </si>
-  <si>
     <t>rối rắm</t>
   </si>
   <si>
@@ -187,6 +178,15 @@
   </si>
   <si>
     <t>cười híp mắt</t>
+  </si>
+  <si>
+    <t>há hốc mồm</t>
+  </si>
+  <si>
+    <t>ha ha</t>
+  </si>
+  <si>
+    <t>nhăn nhó</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -552,34 +552,34 @@
         <v>41</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">

</xml_diff>